<commit_message>
More work on the report
</commit_message>
<xml_diff>
--- a/CVProject/Relazione/sim.xlsx
+++ b/CVProject/Relazione/sim.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcodivincenzo/Documents/Ingegneria/Magistrale/CV/CLion/CVProject/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcodivincenzo/Documents/Ingegneria/Magistrale/CV/CLion/CVProject/Relazione/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F8FD197F-4388-9D4B-8323-6C25D19A4DC4}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{10C604AC-1A69-F247-9E16-C82DB4C83DFE}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17440" xr2:uid="{71D8E087-9B6F-6940-90FB-11258F875A2C}"/>
   </bookViews>
@@ -484,7 +484,7 @@
   <dimension ref="A1:AA36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -959,7 +959,7 @@
       <c r="Q6" s="3">
         <v>0.27777800000000002</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="4">
         <v>26.1111</v>
       </c>
       <c r="S6" s="3">

</xml_diff>